<commit_message>
Added xml schema for exporting as xml
</commit_message>
<xml_diff>
--- a/LibAnswers/LibrarySoftware/SoftwareLists.xlsx
+++ b/LibAnswers/LibrarySoftware/SoftwareLists.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cgalluzzo\Documents\CCACLibraries\Computers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cgalluzzo\Documents\WebSites\libguides\Libguides\public_html\LibAnswers\LibrarySoftware\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,8 +29,25 @@
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="software" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="C:\Users\cgalluzzo\Documents\WebSites\libguides\Libguides\public_html\LibAnswers\LibrarySoftware\software.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="2" name="software1" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="C:\Users\cgalluzzo\Documents\WebSites\libguides\Libguides\public_html\LibAnswers\LibrarySoftware\software.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="3" name="software2" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="C:\Users\cgalluzzo\Documents\WebSites\libguides\Libguides\public_html\LibAnswers\LibrarySoftware\software.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="4" name="software3" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="C:\Users\cgalluzzo\Documents\WebSites\libguides\Libguides\public_html\LibAnswers\LibrarySoftware\software.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="193">
   <si>
     <t>AL-L200-S-01</t>
   </si>
@@ -185,64 +202,430 @@
     <t>HP ScanJet 2000 S2 (document feeder)</t>
   </si>
   <si>
-    <t>AL-L214-S-01</t>
-  </si>
-  <si>
     <t>unavailable</t>
   </si>
   <si>
-    <t>AL-L214-S-02</t>
-  </si>
-  <si>
-    <t>MPC - HC x 64</t>
-  </si>
-  <si>
-    <t>AL-L214-S-03</t>
-  </si>
-  <si>
-    <t>AL-L214-S-04</t>
-  </si>
-  <si>
-    <t>AL-L214-S-05</t>
-  </si>
-  <si>
-    <t>Adobe Acrobat DC</t>
-  </si>
-  <si>
-    <t>AL-L214-S-06</t>
-  </si>
-  <si>
-    <t>AL-L214-S-07</t>
-  </si>
-  <si>
-    <t>AL-L214-S-08</t>
-  </si>
-  <si>
-    <t>AL-L214-S-09</t>
-  </si>
-  <si>
-    <t>AL-L214-S-10</t>
-  </si>
-  <si>
-    <t>AL-L214-S-11</t>
-  </si>
-  <si>
-    <t>AL-L214-S-12</t>
-  </si>
-  <si>
-    <t>AL-L214-S-13</t>
-  </si>
-  <si>
-    <t>AL-L214-S-14</t>
-  </si>
-  <si>
-    <t>AL-L214-S-15</t>
-  </si>
-  <si>
-    <t>AL-L214-S-16</t>
-  </si>
-  <si>
-    <t>AL-L214-S-17</t>
+    <t>AL-L200-S-21</t>
+  </si>
+  <si>
+    <t>AL-L200-S-22</t>
+  </si>
+  <si>
+    <t>AL-L200-S-23</t>
+  </si>
+  <si>
+    <t>AL-L200-S-24</t>
+  </si>
+  <si>
+    <t>AL-L200-S-25</t>
+  </si>
+  <si>
+    <t>AL-L200-S-26</t>
+  </si>
+  <si>
+    <t>AL-L200-S-27</t>
+  </si>
+  <si>
+    <t>AL-L200-S-28</t>
+  </si>
+  <si>
+    <t>AL-L200-S-29</t>
+  </si>
+  <si>
+    <t>AL-L200-S-30</t>
+  </si>
+  <si>
+    <t>AL-L200-S-31</t>
+  </si>
+  <si>
+    <t>AL-L200-S-32</t>
+  </si>
+  <si>
+    <t>AL-L200-S-33</t>
+  </si>
+  <si>
+    <t>AL-L200-S-34</t>
+  </si>
+  <si>
+    <t>AL-L200-S-35</t>
+  </si>
+  <si>
+    <t>AL-L200-S-36</t>
+  </si>
+  <si>
+    <t>AL-L200-S-37</t>
+  </si>
+  <si>
+    <t>AL-L200-S-38</t>
+  </si>
+  <si>
+    <t>AL-L200-S-39</t>
+  </si>
+  <si>
+    <t>AL-L200-S-40</t>
+  </si>
+  <si>
+    <t>AL-L200-S-41</t>
+  </si>
+  <si>
+    <t>AL-L200-S-42</t>
+  </si>
+  <si>
+    <t>AL-L200-S-43</t>
+  </si>
+  <si>
+    <t>AL-L200-S-44</t>
+  </si>
+  <si>
+    <t>AL-L200-S-45</t>
+  </si>
+  <si>
+    <t>AL-L200-S-46</t>
+  </si>
+  <si>
+    <t>AL-L200-S-47</t>
+  </si>
+  <si>
+    <t>AL-L200-S-48</t>
+  </si>
+  <si>
+    <t>AL-L200-S-49</t>
+  </si>
+  <si>
+    <t>AL-L200-S-50</t>
+  </si>
+  <si>
+    <t>AL-L200-S-51</t>
+  </si>
+  <si>
+    <t>AL-L200-S-52</t>
+  </si>
+  <si>
+    <t>AL-L200-S-53</t>
+  </si>
+  <si>
+    <t>AL-L200-S-54</t>
+  </si>
+  <si>
+    <t>AL-L200-S-55</t>
+  </si>
+  <si>
+    <t>AL-L200-S-56</t>
+  </si>
+  <si>
+    <t>AL-L200-S-57</t>
+  </si>
+  <si>
+    <t>AL-L200-S-58</t>
+  </si>
+  <si>
+    <t>AL-L200-S-59</t>
+  </si>
+  <si>
+    <t>AL-L200-S-60</t>
+  </si>
+  <si>
+    <t>AL-L200-S-61</t>
+  </si>
+  <si>
+    <t>AL-L200-S-62</t>
+  </si>
+  <si>
+    <t>AL-L200-S-63</t>
+  </si>
+  <si>
+    <t>AL-L200-S-64</t>
+  </si>
+  <si>
+    <t>AL-L200-S-65</t>
+  </si>
+  <si>
+    <t>AL-L200-S-66</t>
+  </si>
+  <si>
+    <t>AL-L200-S-67</t>
+  </si>
+  <si>
+    <t>AL-L200-S-68</t>
+  </si>
+  <si>
+    <t>AL-L200-S-69</t>
+  </si>
+  <si>
+    <t>AL-L200-S-70</t>
+  </si>
+  <si>
+    <t>AL-L200-S-71</t>
+  </si>
+  <si>
+    <t>AL-L200-S-72</t>
+  </si>
+  <si>
+    <t>AL-L200-S-73</t>
+  </si>
+  <si>
+    <t>AL-L200-S-74</t>
+  </si>
+  <si>
+    <t>AL-L200-S-75</t>
+  </si>
+  <si>
+    <t>AL-L200-S-76</t>
+  </si>
+  <si>
+    <t>AL-L200-S-77</t>
+  </si>
+  <si>
+    <t>AL-L200-S-78</t>
+  </si>
+  <si>
+    <t>AL-L200-S-79</t>
+  </si>
+  <si>
+    <t>AL-L200-S-80</t>
+  </si>
+  <si>
+    <t>AL-L200-S-81</t>
+  </si>
+  <si>
+    <t>AL-L200-S-82</t>
+  </si>
+  <si>
+    <t>AL-L200-S-83</t>
+  </si>
+  <si>
+    <t>AL-L200-S-84</t>
+  </si>
+  <si>
+    <t>AL-L200-S-85</t>
+  </si>
+  <si>
+    <t>AL-L200-S-86</t>
+  </si>
+  <si>
+    <t>AL-L200-S-87</t>
+  </si>
+  <si>
+    <t>AL-L200-S-88</t>
+  </si>
+  <si>
+    <t>AL-L200-S-89</t>
+  </si>
+  <si>
+    <t>AL-L200-S-90</t>
+  </si>
+  <si>
+    <t>AL-L200-S-91</t>
+  </si>
+  <si>
+    <t>AL-L200-S-92</t>
+  </si>
+  <si>
+    <t>AL-L200-S-93</t>
+  </si>
+  <si>
+    <t>AL-L200-S-94</t>
+  </si>
+  <si>
+    <t>AL-L200-S-95</t>
+  </si>
+  <si>
+    <t>AL-L200-S-96</t>
+  </si>
+  <si>
+    <t>AL-L200-S-97</t>
+  </si>
+  <si>
+    <t>AL-L200-S-98</t>
+  </si>
+  <si>
+    <t>AL-L200-S-99</t>
+  </si>
+  <si>
+    <t>AL-L200-S-100</t>
+  </si>
+  <si>
+    <t>AL-L200-S-101</t>
+  </si>
+  <si>
+    <t>AL-L200-S-102</t>
+  </si>
+  <si>
+    <t>AL-L200-S-103</t>
+  </si>
+  <si>
+    <t>AL-L200-S-104</t>
+  </si>
+  <si>
+    <t>AL-L200-S-105</t>
+  </si>
+  <si>
+    <t>AL-L200-S-106</t>
+  </si>
+  <si>
+    <t>AL-L200-S-107</t>
+  </si>
+  <si>
+    <t>AL-L200-S-108</t>
+  </si>
+  <si>
+    <t>AL-L200-S-109</t>
+  </si>
+  <si>
+    <t>AL-L200-S-110</t>
+  </si>
+  <si>
+    <t>AL-L200-S-111</t>
+  </si>
+  <si>
+    <t>AL-L200-S-112</t>
+  </si>
+  <si>
+    <t>AL-L200-S-113</t>
+  </si>
+  <si>
+    <t>AL-L200-S-114</t>
+  </si>
+  <si>
+    <t>AL-L200-S-115</t>
+  </si>
+  <si>
+    <t>AL-L200-S-116</t>
+  </si>
+  <si>
+    <t>AL-L200-S-117</t>
+  </si>
+  <si>
+    <t>AL-L200-S-118</t>
+  </si>
+  <si>
+    <t>AL-L200-S-119</t>
+  </si>
+  <si>
+    <t>AL-L200-S-120</t>
+  </si>
+  <si>
+    <t>AL-L200-S-121</t>
+  </si>
+  <si>
+    <t>AL-L200-S-122</t>
+  </si>
+  <si>
+    <t>AL-L200-S-123</t>
+  </si>
+  <si>
+    <t>AL-L200-S-124</t>
+  </si>
+  <si>
+    <t>AL-L200-S-125</t>
+  </si>
+  <si>
+    <t>AL-L200-S-126</t>
+  </si>
+  <si>
+    <t>AL-L200-S-127</t>
+  </si>
+  <si>
+    <t>AL-L200-S-128</t>
+  </si>
+  <si>
+    <t>AL-L200-S-129</t>
+  </si>
+  <si>
+    <t>AL-L200-S-130</t>
+  </si>
+  <si>
+    <t>AL-L200-S-131</t>
+  </si>
+  <si>
+    <t>AL-L200-S-132</t>
+  </si>
+  <si>
+    <t>AL-L200-S-133</t>
+  </si>
+  <si>
+    <t>AL-L200-S-134</t>
+  </si>
+  <si>
+    <t>AL-L200-S-135</t>
+  </si>
+  <si>
+    <t>AL-L200-S-136</t>
+  </si>
+  <si>
+    <t>AL-L200-S-137</t>
+  </si>
+  <si>
+    <t>AL-L200-S-138</t>
+  </si>
+  <si>
+    <t>AL-L200-S-139</t>
+  </si>
+  <si>
+    <t>AL-L200-S-140</t>
+  </si>
+  <si>
+    <t>AL-L200-S-141</t>
+  </si>
+  <si>
+    <t>AL-L200-S-142</t>
+  </si>
+  <si>
+    <t>AL-L200-S-143</t>
+  </si>
+  <si>
+    <t>AL-L200-S-144</t>
+  </si>
+  <si>
+    <t>AL-L200-S-145</t>
+  </si>
+  <si>
+    <t>AL-L200-S-146</t>
+  </si>
+  <si>
+    <t>AL-L200-S-147</t>
+  </si>
+  <si>
+    <t>AL-L200-S-148</t>
+  </si>
+  <si>
+    <t>AL-L200-S-149</t>
+  </si>
+  <si>
+    <t>AL-L200-S-150</t>
+  </si>
+  <si>
+    <t>AL-L200-S-151</t>
+  </si>
+  <si>
+    <t>AL-L200-S-152</t>
+  </si>
+  <si>
+    <t>AL-L200-S-153</t>
+  </si>
+  <si>
+    <t>AL-L200-S-154</t>
+  </si>
+  <si>
+    <t>AL-L200-S-155</t>
+  </si>
+  <si>
+    <t>AL-L200-S-156</t>
+  </si>
+  <si>
+    <t>AL-L200-S-157</t>
+  </si>
+  <si>
+    <t>AL-L200-S-158</t>
+  </si>
+  <si>
+    <t>AL-L200-S-159</t>
+  </si>
+  <si>
+    <t>AL-L200-S-160</t>
+  </si>
+  <si>
+    <t>AL-L200-S-161</t>
   </si>
 </sst>
 </file>
@@ -295,7 +678,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -316,11 +699,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -331,6 +731,33 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/xmlMaps.xml><?xml version="1.0" encoding="utf-8"?>
+<MapInfo xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" SelectionNamespaces="">
+  <Schema ID="Schema4">
+    <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
+      <xsd:element nillable="true" name="software">
+        <xsd:complexType>
+          <xsd:sequence minOccurs="0">
+            <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="item" form="unqualified">
+              <xsd:complexType>
+                <xsd:sequence minOccurs="0">
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="computer" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="resource" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="campus" form="unqualified"/>
+                </xsd:sequence>
+              </xsd:complexType>
+            </xsd:element>
+          </xsd:sequence>
+        </xsd:complexType>
+      </xsd:element>
+    </xsd:schema>
+  </Schema>
+  <Map ID="4" Name="software_Map" RootElement="software" SchemaID="Schema4" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+    <DataBinding FileBinding="true" ConnectionID="4" DataBindingLoadMode="1"/>
+  </Map>
+</MapInfo>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1305,6 +1732,24 @@
     </ext>
   </extLst>
 </pivotTableDefinition>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:C147" tableType="xml" totalsRowShown="0" headerRowDxfId="2" connectionId="4">
+  <autoFilter ref="A1:C147"/>
+  <tableColumns count="3">
+    <tableColumn id="1" uniqueName="computer" name="AL-L200-S-15" dataDxfId="3">
+      <xmlColumnPr mapId="4" xpath="/software/item/computer" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="2" uniqueName="resource" name="Adobe Creative Cloud" dataDxfId="1">
+      <xmlColumnPr mapId="4" xpath="/software/item/resource" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="3" uniqueName="campus" name="Allegheny" dataDxfId="0">
+      <xmlColumnPr mapId="4" xpath="/software/item/campus" xmlDataType="string"/>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2706,7 +3151,7 @@
         <v>&lt;tr&gt;&lt;td&gt;Respondus Lockdown Browser&lt;/td&gt;&lt;td&gt;AL-L200-S-14&lt;/td&gt;&lt;td&gt;Allegheny&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="76" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>27</v>
       </c>
@@ -2721,7 +3166,7 @@
         <v>&lt;tr&gt;&lt;td&gt;Respondus Lockdown Browser&lt;/td&gt;&lt;td&gt;AL-L200-S-16&lt;/td&gt;&lt;td&gt;Allegheny&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="77" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>28</v>
       </c>
@@ -2736,7 +3181,7 @@
         <v>&lt;tr&gt;&lt;td&gt;Respondus Lockdown Browser&lt;/td&gt;&lt;td&gt;AL-L200-S-17&lt;/td&gt;&lt;td&gt;Allegheny&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="78" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>29</v>
       </c>
@@ -2751,7 +3196,7 @@
         <v>&lt;tr&gt;&lt;td&gt;Respondus Lockdown Browser&lt;/td&gt;&lt;td&gt;AL-L200-S-18&lt;/td&gt;&lt;td&gt;Allegheny&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="79" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>31</v>
       </c>
@@ -2823,1840 +3268,1844 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D147"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:C147"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.5703125" customWidth="1"/>
     <col min="2" max="2" width="33.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B1" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>35</v>
+      <c r="A3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="A4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="A5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="A6" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="A7" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="A8" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="A9" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="A10" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="A11" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="A12" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="A13" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="A14" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="A15" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="A16" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="A17" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="A18" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="A19" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="A20" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="A21" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="A22" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="A23" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>8</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>9</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="A24" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="A27" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>37</v>
-      </c>
-      <c r="B29" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>36</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C30" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>9</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C31" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>0</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C32" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>1</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C33" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>2</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C34" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>3</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C35" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>4</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C36" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>5</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C37" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>6</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="A29" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>7</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="A39" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C39" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C40" t="s">
+      <c r="A40" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>30</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="A41" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>31</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C42" t="s">
+      <c r="A42" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>0</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="A43" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>1</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C44" t="s">
+      <c r="A44" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C44" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>2</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C45" t="s">
+      <c r="A45" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>3</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C46" t="s">
+      <c r="A46" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C46" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>4</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C47" t="s">
+      <c r="A47" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C47" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>5</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C48" t="s">
+      <c r="A48" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C48" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>6</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C49" t="s">
+      <c r="A49" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C49" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>7</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C50" t="s">
+      <c r="A50" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C50" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>8</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C51" t="s">
+      <c r="A51" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C51" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>0</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="A52" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C52" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>1</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C53" t="s">
+      <c r="A53" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C53" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>2</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C54" t="s">
+      <c r="A54" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C54" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>3</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C55" t="s">
+      <c r="A55" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C55" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>4</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C56" t="s">
+      <c r="A56" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C56" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>5</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C57" t="s">
+      <c r="A57" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C57" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>6</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C58" t="s">
+      <c r="A58" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C58" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>7</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C59" t="s">
+      <c r="A59" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C59" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>8</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C60" t="s">
+      <c r="A60" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C60" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>0</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C61" t="s">
+      <c r="A61" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C61" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>1</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C62" t="s">
+      <c r="A62" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C62" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>2</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C63" t="s">
+      <c r="A63" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C63" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>3</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C64" t="s">
+      <c r="A64" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C64" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>4</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C65" t="s">
+      <c r="A65" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C65" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>5</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C66" t="s">
+      <c r="A66" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C66" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>6</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C67" t="s">
+      <c r="A67" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C67" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>7</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C68" t="s">
+      <c r="A68" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C68" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>8</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C69" t="s">
+      <c r="A69" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C69" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>9</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C70" t="s">
+      <c r="A70" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C70" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>10</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C71" t="s">
+      <c r="A71" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C71" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>11</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C72" t="s">
+      <c r="A72" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B72" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C72" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>12</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C73" t="s">
+      <c r="A73" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B73" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C73" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>13</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C74" t="s">
+      <c r="A74" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B74" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C74" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>27</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C75" t="s">
+      <c r="A75" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B75" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C75" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>31</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C76" t="s">
+      <c r="A76" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B76" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C76" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>42</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C77" t="s">
+      <c r="A77" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B77" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C77" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>40</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C78" t="s">
+      <c r="A78" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B78" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C78" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>41</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C79" t="s">
+      <c r="A79" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B79" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C79" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+      <c r="A80" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B80" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C80" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D80" t="s">
         <v>51</v>
       </c>
-      <c r="B80" t="s">
-        <v>32</v>
-      </c>
-      <c r="C80" t="s">
-        <v>33</v>
-      </c>
-      <c r="D80" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>53</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C81" t="s">
+      <c r="A81" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B81" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C81" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D81" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>53</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C82" t="s">
+      <c r="A82" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C82" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D82" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>53</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C83" t="s">
+      <c r="A83" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B83" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C83" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D83" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>55</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C84" t="s">
+      <c r="A84" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B84" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C84" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D84" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>55</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C85" t="s">
+      <c r="A85" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B85" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C85" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D85" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>55</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C86" t="s">
+      <c r="A86" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B86" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C86" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D86" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>56</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C87" t="s">
+      <c r="A87" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B87" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C87" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D87" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>56</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C88" t="s">
+      <c r="A88" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B88" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C88" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D88" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>56</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C89" t="s">
+      <c r="A89" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B89" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C89" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D89" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>57</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C90" t="s">
+      <c r="A90" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B90" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C90" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D90" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>57</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C91" t="s">
+      <c r="A91" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B91" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C91" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D91" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>57</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C92" t="s">
+      <c r="A92" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B92" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C92" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D92" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>57</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C93" t="s">
+      <c r="A93" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="B93" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C93" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D93" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>57</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C94" t="s">
+      <c r="A94" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B94" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C94" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D94" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>59</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C95" t="s">
+      <c r="A95" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="B95" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C95" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D95" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>59</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C96" t="s">
+      <c r="A96" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="B96" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C96" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D96" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>59</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C97" t="s">
+      <c r="A97" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B97" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C97" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D97" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>60</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C98" t="s">
+      <c r="A98" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="B98" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C98" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D98" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>60</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C99" t="s">
+      <c r="A99" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="B99" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C99" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D99" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>60</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C100" t="s">
+      <c r="A100" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B100" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C100" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D100" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>60</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C101" t="s">
+      <c r="A101" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="B101" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C101" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D101" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>60</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C102" t="s">
+      <c r="A102" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="B102" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C102" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D102" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>61</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C103" t="s">
+      <c r="A103" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="B103" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C103" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D103" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>61</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C104" t="s">
+      <c r="A104" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B104" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C104" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D104" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>61</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C105" t="s">
+      <c r="A105" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B105" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C105" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D105" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>61</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C106" t="s">
+      <c r="A106" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B106" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C106" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D106" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>61</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C107" t="s">
+      <c r="A107" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B107" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C107" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D107" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>62</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C108" t="s">
+      <c r="A108" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="B108" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C108" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D108" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>62</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C109" t="s">
+      <c r="A109" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B109" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C109" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D109" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>62</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C110" t="s">
+      <c r="A110" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B110" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C110" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D110" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>62</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C111" t="s">
+      <c r="A111" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="B111" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C111" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D111" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>62</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C112" t="s">
+      <c r="A112" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B112" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C112" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D112" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>63</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C113" t="s">
+      <c r="A113" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B113" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C113" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D113" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>63</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C114" t="s">
+      <c r="A114" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B114" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C114" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D114" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>63</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C115" t="s">
+      <c r="A115" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="B115" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C115" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D115" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>63</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C116" t="s">
+      <c r="A116" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B116" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C116" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D116" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>63</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C117" t="s">
+      <c r="A117" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B117" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C117" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D117" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>63</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C118" t="s">
+      <c r="A118" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B118" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C118" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D118" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>64</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C119" t="s">
+      <c r="A119" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B119" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C119" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D119" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>64</v>
-      </c>
-      <c r="B120" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C120" t="s">
+      <c r="A120" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B120" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C120" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D120" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>64</v>
-      </c>
-      <c r="B121" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C121" t="s">
+      <c r="A121" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="B121" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C121" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D121" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>64</v>
-      </c>
-      <c r="B122" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C122" t="s">
+      <c r="A122" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B122" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C122" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D122" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>65</v>
-      </c>
-      <c r="B123" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C123" t="s">
+      <c r="A123" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B123" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C123" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D123" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>65</v>
-      </c>
-      <c r="B124" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C124" t="s">
+      <c r="A124" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B124" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C124" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D124" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>65</v>
-      </c>
-      <c r="B125" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C125" t="s">
+      <c r="A125" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="B125" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C125" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D125" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>65</v>
-      </c>
-      <c r="B126" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C126" t="s">
+      <c r="A126" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B126" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C126" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D126" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>65</v>
-      </c>
-      <c r="B127" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C127" t="s">
+      <c r="A127" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="B127" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C127" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D127" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>66</v>
-      </c>
-      <c r="B128" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C128" t="s">
+      <c r="A128" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B128" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C128" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D128" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>66</v>
-      </c>
-      <c r="B129" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C129" t="s">
+      <c r="A129" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="B129" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C129" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D129" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>66</v>
-      </c>
-      <c r="B130" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C130" t="s">
+      <c r="A130" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="B130" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C130" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D130" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>66</v>
-      </c>
-      <c r="B131" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C131" t="s">
+      <c r="A131" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B131" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C131" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D131" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>67</v>
-      </c>
-      <c r="B132" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C132" t="s">
+      <c r="A132" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B132" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C132" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D132" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>67</v>
-      </c>
-      <c r="B133" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C133" t="s">
+      <c r="A133" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="B133" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C133" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D133" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>67</v>
-      </c>
-      <c r="B134" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C134" t="s">
+      <c r="A134" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B134" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C134" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D134" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>67</v>
-      </c>
-      <c r="B135" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C135" t="s">
+      <c r="A135" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="B135" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C135" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D135" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>68</v>
-      </c>
-      <c r="B136" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C136" t="s">
+      <c r="A136" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="B136" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C136" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D136" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>68</v>
-      </c>
-      <c r="B137" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C137" t="s">
+      <c r="A137" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="B137" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C137" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D137" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>68</v>
-      </c>
-      <c r="B138" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C138" t="s">
+      <c r="A138" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B138" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C138" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D138" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>68</v>
-      </c>
-      <c r="B139" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C139" t="s">
+      <c r="A139" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="B139" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C139" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D139" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>69</v>
-      </c>
-      <c r="B140" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C140" t="s">
+      <c r="A140" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B140" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C140" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D140" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>69</v>
-      </c>
-      <c r="B141" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C141" t="s">
+      <c r="A141" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="B141" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C141" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D141" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>69</v>
-      </c>
-      <c r="B142" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C142" t="s">
+      <c r="A142" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="B142" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C142" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D142" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>69</v>
-      </c>
-      <c r="B143" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C143" t="s">
+      <c r="A143" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="B143" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C143" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D143" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>70</v>
-      </c>
-      <c r="B144" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C144" t="s">
+      <c r="A144" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="B144" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C144" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D144" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>70</v>
-      </c>
-      <c r="B145" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C145" t="s">
+      <c r="A145" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="B145" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C145" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D145" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>70</v>
-      </c>
-      <c r="B146" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C146" t="s">
+      <c r="A146" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="B146" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C146" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D146" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
-        <v>70</v>
-      </c>
-      <c r="B147" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C147" t="s">
+      <c r="A147" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="B147" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C147" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D147" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>